<commit_message>
Feature: SS 9-16, 21-78 / NBDS 1-5 / NS 700 (graphics by Voyager One) (issue #3952)
</commit_message>
<xml_diff>
--- a/docs/steamtrains_overview.xlsx
+++ b/docs/steamtrains_overview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="291">
   <si>
     <t>NS</t>
   </si>
@@ -661,9 +661,6 @@
   </si>
   <si>
     <t>last service</t>
-  </si>
-  <si>
-    <t>1867</t>
   </si>
   <si>
     <t>1933</t>
@@ -1243,8 +1240,8 @@
   <dimension ref="A1:Q124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1294,7 @@
         <v>214</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>86</v>
@@ -1330,16 +1327,16 @@
         <v>116</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="O4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>183</v>
@@ -1361,16 +1358,16 @@
         <v>93</v>
       </c>
       <c r="M6" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>183</v>
@@ -1384,19 +1381,19 @@
         <v>184</v>
       </c>
       <c r="M7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="O7" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1407,19 +1404,19 @@
         <v>185</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="O8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1444,19 +1441,19 @@
         <v>152</v>
       </c>
       <c r="M10" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="O10" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1470,19 +1467,19 @@
         <v>162</v>
       </c>
       <c r="M11" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="P11" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1499,19 +1496,19 @@
         <v>176</v>
       </c>
       <c r="M12" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="O12" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1538,19 +1535,19 @@
         <v>111</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1561,19 +1558,19 @@
         <v>136</v>
       </c>
       <c r="M16" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="P16" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1598,19 +1595,19 @@
         <v>188</v>
       </c>
       <c r="M18" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="P18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1621,19 +1618,19 @@
         <v>204</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N19" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="P19" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1660,19 +1657,19 @@
         <v>191</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O22" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q22" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1683,19 +1680,19 @@
         <v>137</v>
       </c>
       <c r="M23" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="O23" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1706,19 +1703,19 @@
         <v>138</v>
       </c>
       <c r="M24" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="N24" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="O24" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1734,19 +1731,19 @@
         <v>157</v>
       </c>
       <c r="M26" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="N26" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="N26" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="O26" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1765,19 +1762,19 @@
         <v>165</v>
       </c>
       <c r="M28" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="O28" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1788,19 +1785,19 @@
         <v>192</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -1816,19 +1813,19 @@
         <v>193</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -1839,19 +1836,19 @@
         <v>193</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -1918,19 +1915,19 @@
         <v>193</v>
       </c>
       <c r="M43" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="O43" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="N43" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="P43" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -1951,19 +1948,19 @@
         <v>193</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O46" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="P46" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="P46" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="Q46" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -1987,19 +1984,19 @@
         <v>129</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P49" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q49" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -2016,16 +2013,16 @@
         <v>177</v>
       </c>
       <c r="M50" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="N50" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="N50" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="O50" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>183</v>
@@ -2048,16 +2045,16 @@
         <v>180</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>183</v>
@@ -2074,19 +2071,19 @@
         <v>164</v>
       </c>
       <c r="M52" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="N52" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="N52" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="O52" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -2097,16 +2094,16 @@
         <v>139</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>183</v>
@@ -2123,19 +2120,19 @@
         <v>161</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P54" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q54" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q54" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -2151,19 +2148,19 @@
         <v>140</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P56" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q56" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q56" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -2205,10 +2202,10 @@
         <v>113</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q62" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -2219,19 +2216,19 @@
         <v>193</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -2258,19 +2255,19 @@
         <v>181</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q66" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -2300,19 +2297,19 @@
         <v>156</v>
       </c>
       <c r="M69" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="N69" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="N69" s="2" t="s">
+      <c r="O69" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="O69" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="P69" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q69" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q69" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -2326,19 +2323,19 @@
         <v>163</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -2355,19 +2352,19 @@
         <v>167</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -2381,19 +2378,19 @@
         <v>200</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q72" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -2407,19 +2404,19 @@
         <v>166</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -2430,19 +2427,19 @@
         <v>145</v>
       </c>
       <c r="M74" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="N74" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="N74" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="O74" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P74" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q74" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q74" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -2461,19 +2458,19 @@
         <v>115</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P76" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q76" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q76" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -2492,19 +2489,19 @@
         <v>203</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P78" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q78" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -2515,19 +2512,19 @@
         <v>203</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q79" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -2541,19 +2538,19 @@
         <v>159</v>
       </c>
       <c r="M80" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="N80" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="O80" s="2" t="s">
         <v>125</v>
       </c>
       <c r="P80" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q80" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -2564,19 +2561,19 @@
         <v>108</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q81" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -2639,19 +2636,19 @@
         <v>203</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q87" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
@@ -2662,19 +2659,19 @@
         <v>203</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q88" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
@@ -2685,16 +2682,16 @@
         <v>203</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -2705,19 +2702,19 @@
         <v>203</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
@@ -2728,19 +2725,19 @@
         <v>203</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>